<commit_message>
generate code by ai
</commit_message>
<xml_diff>
--- a/src/main/resources/test_excel.xlsx
+++ b/src/main/resources/test_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yupi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lv jiang er hao\Desktop\java\git\wisdom\wisdom-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF756E6F-D024-F543-BF1B-5BFCE872F8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97C1BA5-8B72-472C-8DDB-6E01D326CB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="2660" windowWidth="28060" windowHeight="16940" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,21 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>小数</t>
+    <t>年份</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>日期</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>整数</t>
-  </si>
-  <si>
-    <t>字符串</t>
+    <t>销售额</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -57,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -115,17 +107,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -440,43 +433,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260829AF-83D5-9D43-A57C-13A2BDCFFDE0}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="22.8"/>
   <cols>
-    <col min="4" max="4" width="10.77734375" style="5"/>
+    <col min="4" max="4" width="10.75" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="3">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="C2" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44844</v>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>